<commit_message>
Big cleanup in main file.
</commit_message>
<xml_diff>
--- a/Data/Urbanisation2010.xlsx
+++ b/Data/Urbanisation2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\Dissertation\Migration\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C741672-7491-4282-AB80-1497A84C678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C432FE6A-840C-4F35-A5A5-036F38326FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{774F95F9-8A58-434E-94F2-85EB387A060B}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{774F95F9-8A58-434E-94F2-85EB387A060B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Johor</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Pulau Pinang</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -138,31 +141,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -517,151 +515,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063E1E62-BECF-4CAB-88D8-BA46B2E52954}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>71.745396911875787</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>64.369225230043298</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>41.666870651718639</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>86.468785120536211</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>66.595248041987247</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="5">
         <v>50.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>90.711932722017082</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6">
         <v>69.353952153043466</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="7">
         <v>51.342906528387175</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="8">
         <v>91.335553537641516</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="8">
         <v>59.334976660210039</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7">
         <v>53.245118937064639</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="7">
         <v>53.712811567776008</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="7">
         <v>81.900000000000006</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>100</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="9">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>67.3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9">
+        <v>44.1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>90.9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="9">
+        <v>69.3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>52.8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="9">
+        <v>92.5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="9">
+        <v>53.8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1">
+        <v>96.8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="9">
+        <v>64.2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1">
+        <v>54.7</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1">
+        <v>88.9</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1">
+        <v>100</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>